<commit_message>
CGC-12, CGC-13, CGC-14, CGC-15
</commit_message>
<xml_diff>
--- a/public/uploads/invoice/invoice-1.xlsx
+++ b/public/uploads/invoice/invoice-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>INVOICE</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Office: 404-684-5963</t>
   </si>
   <si>
-    <t>07/07/2024</t>
+    <t>12/20/2024</t>
   </si>
   <si>
     <t>East Point, Ga. 30344</t>
@@ -87,10 +87,10 @@
     <t>Inspector's Name:</t>
   </si>
   <si>
-    <t>01/06/2024</t>
-  </si>
-  <si>
-    <t>30/06/2024</t>
+    <t>08/01/2024</t>
+  </si>
+  <si>
+    <t>08/31/2024</t>
   </si>
   <si>
     <t>CONTRACTOR, INC</t>
@@ -114,13 +114,7 @@
     <t>Contact Name</t>
   </si>
   <si>
-    <t>Dan Schamerhorn</t>
-  </si>
-  <si>
     <t>Email/No.</t>
-  </si>
-  <si>
-    <t>merhorn@earsnel.com</t>
   </si>
   <si>
     <t>gill@arersnl.com</t>
@@ -1360,7 +1354,7 @@
   <dimension ref="A1:N206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="false" showRowColHeaders="1">
-      <selection activeCell="M28" sqref="M28:M28"/>
+      <selection activeCell="M31" sqref="M31:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="15" defaultColWidth="8.83203125" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1520,22 +1514,18 @@
       <c r="B14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="C14" s="13"/>
       <c r="D14" s="68"/>
       <c r="E14" s="69"/>
       <c r="F14" s="70"/>
     </row>
     <row r="15" spans="1:14" customHeight="1" ht="16.5">
       <c r="B15" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="71" t="s">
         <v>26</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="71" t="s">
-        <v>28</v>
       </c>
       <c r="E15" s="72"/>
       <c r="F15" s="73"/>
@@ -1549,30 +1539,30 @@
     </row>
     <row r="17" spans="1:14" customHeight="1" ht="15">
       <c r="B17" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" s="51"/>
       <c r="F17" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G17" s="51" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H17" s="51"/>
     </row>
     <row r="18" spans="1:14" customHeight="1" ht="15">
       <c r="B18" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D18" s="51"/>
       <c r="F18" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G18" s="51">
         <v>896532</v>
@@ -1581,7 +1571,7 @@
     </row>
     <row r="19" spans="1:14" customHeight="1" ht="15">
       <c r="F19" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G19" s="42">
         <v>896532</v>
@@ -1590,7 +1580,7 @@
     </row>
     <row r="20" spans="1:14" customHeight="1" ht="15">
       <c r="A20" s="66" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="32"/>
       <c r="C20" s="33"/>
@@ -1615,39 +1605,39 @@
     <row r="23" spans="1:14" customHeight="1" ht="15"/>
     <row r="24" spans="1:14" customHeight="1" ht="49">
       <c r="A24" s="22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="40"/>
       <c r="D24" s="41"/>
       <c r="E24" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="H24" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="24" t="s">
+      <c r="I24" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="J24" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="I24" s="23" t="s">
+      <c r="K24" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="L24" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="K24" s="23" t="s">
+      <c r="M24" s="23" t="s">
         <v>45</v>
-      </c>
-      <c r="L24" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="M24" s="23" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:14" customHeight="1" ht="15">
@@ -1655,12 +1645,12 @@
         <v>1</v>
       </c>
       <c r="B25" s="80" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="81"/>
       <c r="D25" s="82"/>
       <c r="E25" s="79" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F25" s="83">
         <v>50.0</v>
@@ -1690,12 +1680,12 @@
         <v>2</v>
       </c>
       <c r="B26" s="80" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="81"/>
       <c r="D26" s="82"/>
       <c r="E26" s="79" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F26" s="83">
         <v>60.0</v>
@@ -1725,12 +1715,12 @@
         <v>3</v>
       </c>
       <c r="B27" s="80" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" s="81"/>
       <c r="D27" s="82"/>
       <c r="E27" s="79" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F27" s="83">
         <v>50.0</v>
@@ -1756,74 +1746,140 @@
       </c>
     </row>
     <row r="28" spans="1:14" customHeight="1" ht="15">
-      <c r="A28" s="79"/>
-      <c r="B28" s="80"/>
+      <c r="A28" s="79">
+        <v>4</v>
+      </c>
+      <c r="B28" s="80" t="s">
+        <v>46</v>
+      </c>
       <c r="C28" s="81"/>
       <c r="D28" s="82"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="88" t="s">
-        <v>53</v>
-      </c>
-      <c r="H28" s="88">
-        <v>35000.0</v>
-      </c>
-      <c r="I28" s="86"/>
-      <c r="J28" s="89" t="s">
-        <v>54</v>
-      </c>
-      <c r="K28" s="86"/>
-      <c r="L28" s="90">
-        <v>25400.0</v>
-      </c>
-      <c r="M28" s="90">
-        <v>25400.0</v>
+      <c r="E28" s="79" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="83">
+        <v>50.0</v>
+      </c>
+      <c r="G28" s="84">
+        <v>160.0</v>
+      </c>
+      <c r="H28" s="84">
+        <v>8000.0</v>
+      </c>
+      <c r="I28" s="86">
+        <v>40.0</v>
+      </c>
+      <c r="J28" s="86">
+        <v>40.0</v>
+      </c>
+      <c r="K28" s="86">
+        <v>80.0</v>
+      </c>
+      <c r="L28" s="87">
+        <v>6400.0</v>
+      </c>
+      <c r="M28" s="87">
+        <v>12800.0</v>
       </c>
     </row>
     <row r="29" spans="1:14" customHeight="1" ht="15">
-      <c r="A29" s="25"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30"/>
+      <c r="A29" s="79">
+        <v>5</v>
+      </c>
+      <c r="B29" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="81"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="83">
+        <v>60.0</v>
+      </c>
+      <c r="G29" s="84">
+        <v>200.0</v>
+      </c>
+      <c r="H29" s="84">
+        <v>12000.0</v>
+      </c>
+      <c r="I29" s="86">
+        <v>50.0</v>
+      </c>
+      <c r="J29" s="86">
+        <v>50.0</v>
+      </c>
+      <c r="K29" s="86">
+        <v>100.0</v>
+      </c>
+      <c r="L29" s="87">
+        <v>10000.0</v>
+      </c>
+      <c r="M29" s="87">
+        <v>20000.0</v>
+      </c>
     </row>
     <row r="30" spans="1:14" customHeight="1" ht="15">
-      <c r="A30" s="25"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
+      <c r="A30" s="79">
+        <v>6</v>
+      </c>
+      <c r="B30" s="80" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="81"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="79" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="83">
+        <v>50.0</v>
+      </c>
+      <c r="G30" s="84">
+        <v>300.0</v>
+      </c>
+      <c r="H30" s="84">
+        <v>15000.0</v>
+      </c>
+      <c r="I30" s="86">
+        <v>30.0</v>
+      </c>
+      <c r="J30" s="86">
+        <v>1.0</v>
+      </c>
+      <c r="K30" s="86">
+        <v>31.0</v>
+      </c>
+      <c r="L30" s="87">
+        <v>300.0</v>
+      </c>
+      <c r="M30" s="87">
+        <v>9300.0</v>
+      </c>
     </row>
     <row r="31" spans="1:14" customHeight="1" ht="15">
-      <c r="A31" s="25"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
+      <c r="A31" s="79"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="83"/>
+      <c r="G31" s="88" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" s="88">
+        <v>70000.0</v>
+      </c>
+      <c r="I31" s="86"/>
+      <c r="J31" s="89" t="s">
+        <v>52</v>
+      </c>
+      <c r="K31" s="86"/>
+      <c r="L31" s="90">
+        <v>42100.0</v>
+      </c>
+      <c r="M31" s="90">
+        <v>67500.0</v>
+      </c>
     </row>
     <row r="32" spans="1:14" customHeight="1" ht="15">
       <c r="A32" s="25"/>
@@ -3880,7 +3936,7 @@
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B38:D38"/>
-    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J31:K31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId_hyperlink_1"/>

</xml_diff>